<commit_message>
Copy brain atrophy data file from Rebecca
</commit_message>
<xml_diff>
--- a/data/raw/Spain Manifest.xlsx
+++ b/data/raw/Spain Manifest.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\OHSU Shared\Restricted\SOM\NEURO\MS Center\LA in MS Program\Glutathione study\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="10">
   <si>
     <t>Patient ID</t>
   </si>
@@ -52,12 +52,18 @@
   <si>
     <t>Sample #</t>
   </si>
+  <si>
+    <t>M24 brain atrophy (% change)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +79,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -82,9 +94,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -94,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -107,11 +128,2101 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="160">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -387,10 +2498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,9 +2510,10 @@
     <col min="2" max="2" width="11.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -414,8 +2526,11 @@
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -428,8 +2543,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6">
+        <v>0.35809150000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -443,7 +2561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -457,7 +2575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -470,8 +2588,11 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="6">
+        <v>-2.0259800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -485,7 +2606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -499,7 +2620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -512,8 +2633,11 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="6">
+        <v>-1.5444500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -527,7 +2651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -540,8 +2664,11 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="6">
+        <v>0.534273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -555,7 +2682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -568,8 +2695,11 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="6">
+        <v>-0.67900550000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -583,7 +2713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -597,7 +2727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -610,8 +2740,11 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="6">
+        <v>0.80429249999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -625,7 +2758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -639,7 +2772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -652,8 +2785,11 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="6">
+        <v>-1.1199600000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -667,7 +2803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -681,7 +2817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -694,8 +2830,11 @@
       <c r="D21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="7">
+        <v>-1.462645</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -709,7 +2848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -723,7 +2862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -736,8 +2875,11 @@
       <c r="D24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="6">
+        <v>0.20021505000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -751,7 +2893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -765,7 +2907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -778,8 +2920,11 @@
       <c r="D27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="6">
+        <v>-1.7466649999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -793,7 +2938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -807,7 +2952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -820,8 +2965,11 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="8">
+        <v>-1.55396</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -835,7 +2983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -849,7 +2997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -862,8 +3010,11 @@
       <c r="D33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="6">
+        <v>0.59592999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -877,7 +3028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -891,7 +3042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -904,8 +3055,11 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="6">
+        <v>-0.26704549999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -919,7 +3073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -933,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -946,8 +3100,11 @@
       <c r="D39" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="6">
+        <v>-2.1748099999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -961,7 +3118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -975,7 +3132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -988,8 +3145,11 @@
       <c r="D42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="6">
+        <v>-1.105561</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1003,7 +3163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1017,7 +3177,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1030,8 +3190,11 @@
       <c r="D45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="6">
+        <v>-1.74343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1045,7 +3208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1059,7 +3222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1072,8 +3235,11 @@
       <c r="D48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="6">
+        <v>-2.01153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -1087,7 +3253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1101,7 +3267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1114,8 +3280,11 @@
       <c r="D51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="6">
+        <v>7.3825950000000001E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1129,7 +3298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1143,7 +3312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1156,8 +3325,11 @@
       <c r="D54" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="6">
+        <v>-0.15640029999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1171,7 +3343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1185,7 +3357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1198,8 +3370,11 @@
       <c r="D57" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="6">
+        <v>-1.2207250000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1213,7 +3388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1228,6 +3403,287 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="159" priority="77" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="158" priority="78" operator="beginsWith" text="4,">
+      <formula>LEFT(E2,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="79" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="156" priority="80" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="151" priority="73" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="150" priority="74" operator="beginsWith" text="4,">
+      <formula>LEFT(E5,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="75" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="148" priority="76" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="143" priority="69" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="142" priority="70" operator="beginsWith" text="4,">
+      <formula>LEFT(E8,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="71" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="72" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="135" priority="65" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="134" priority="66" operator="beginsWith" text="4,">
+      <formula>LEFT(E10,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="67" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="68" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="127" priority="61" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="126" priority="62" operator="beginsWith" text="4,">
+      <formula>LEFT(E12,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="63" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="64" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="119" priority="57" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="118" priority="58" operator="beginsWith" text="4,">
+      <formula>LEFT(E15,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="59" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="60" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="111" priority="53" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="110" priority="54" operator="beginsWith" text="4,">
+      <formula>LEFT(E18,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="55" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="56" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="103" priority="49" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="102" priority="50" operator="beginsWith" text="4,">
+      <formula>LEFT(E21,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="51" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="52" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="95" priority="45" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="94" priority="46" operator="beginsWith" text="4,">
+      <formula>LEFT(E24,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="47" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="48" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="87" priority="41" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="86" priority="42" operator="beginsWith" text="4,">
+      <formula>LEFT(E27,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="43" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="44" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="79" priority="37" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="78" priority="38" operator="beginsWith" text="4,">
+      <formula>LEFT(E30,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="40" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="cellIs" dxfId="71" priority="33" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="70" priority="34" operator="beginsWith" text="4,">
+      <formula>LEFT(E33,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="35" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="36" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="62" priority="30" operator="beginsWith" text="4,">
+      <formula>LEFT(E36,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="31" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="32" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="55" priority="25" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="54" priority="26" operator="beginsWith" text="4,">
+      <formula>LEFT(E39,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="27" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="28" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" dxfId="47" priority="21" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="46" priority="22" operator="beginsWith" text="4,">
+      <formula>LEFT(E42,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="24" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="38" priority="18" operator="beginsWith" text="4,">
+      <formula>LEFT(E45,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="20" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="30" priority="14" operator="beginsWith" text="4,">
+      <formula>LEFT(E48,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="16" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="22" priority="10" operator="beginsWith" text="4,">
+      <formula>LEFT(E51,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="6" operator="beginsWith" text="4,">
+      <formula>LEFT(E54,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="4,">
+      <formula>LEFT(E57,LEN("4,"))="4,"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="3,">
+      <formula>NOT(ISERROR(SEARCH("3,",E57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>